<commit_message>
fix: import excel with jam pelajaran
</commit_message>
<xml_diff>
--- a/public/templates/template_guru.xlsx
+++ b/public/templates/template_guru.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridzimeko\Documents\Projects\jadwal-azmania\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D97D9A-CB96-4EA0-AF46-015A35F8A2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88880B5-9DDB-4652-8D8B-5F7556FFD3EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="1620" windowWidth="15240" windowHeight="9300" xr2:uid="{B6CCB068-24C6-409C-8CDA-B41A8E75B8E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B6CCB068-24C6-409C-8CDA-B41A8E75B8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Nama Guru</t>
   </si>
   <si>
     <t>Kode Guru</t>
+  </si>
+  <si>
+    <t>Warna</t>
   </si>
 </sst>
 </file>
@@ -446,14 +449,14 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -463,7 +466,9 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>

</xml_diff>